<commit_message>
Modified And Added Final Table for 2018
</commit_message>
<xml_diff>
--- a/report-2018/injuries_report-q1_2018.xlsx
+++ b/report-2018/injuries_report-q1_2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataSet\Open Data\injuries_report\report-2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataSet\Open Data\Injuries_Reports\report-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BD3D43-B2D1-4D26-9DC2-FC9AD7AAFD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E105AA4-5769-41A9-B239-8950941EE219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="743" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="743" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T1_Q1_2018" sheetId="6" r:id="rId1"/>
@@ -1202,39 +1202,6 @@
         <name val="Sakkal Majalla"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1286,379 +1253,6 @@
           <color theme="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC1D9CE"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2088,19 +1682,37 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2125,7 +1737,7 @@
           <bgColor rgb="FFC1D9CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="1"/>
@@ -2153,7 +1765,57 @@
         <name val="Sakkal Majalla"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2585,16 +2247,150 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC1D9CE"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
         <top style="thin">
           <color theme="1"/>
         </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2817,50 +2613,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFA7C9BA"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2879,7 +2641,57 @@
         <name val="Sakkal Majalla"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3101,19 +2913,37 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3135,10 +2965,10 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFBFD7CD"/>
+          <bgColor rgb="FFA7C9BA"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="1"/>
@@ -3148,62 +2978,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3252,14 +3026,14 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="16"/>
         <color indexed="8"/>
         <name val="Sakkal Majalla"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="1"/>
         </left>
@@ -3272,398 +3046,7 @@
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBFD7CD"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Sakkal Majalla"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4093,9 +3476,567 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBFD7CD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4106,6 +4047,65 @@
         <top style="thin">
           <color theme="1"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Sakkal Majalla"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBFD7CD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -4122,126 +4122,126 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEB3C82F-E60D-4711-BB4E-51719D11C854}" name="Table2" displayName="Table2" ref="A1:N23" totalsRowShown="0" headerRowDxfId="62" dataDxfId="63" headerRowBorderDxfId="76" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEB3C82F-E60D-4711-BB4E-51719D11C854}" name="Table2" displayName="Table2" ref="A1:N23" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90">
   <autoFilter ref="A1:N23" xr:uid="{EEB3C82F-E60D-4711-BB4E-51719D11C854}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{AD06DBA2-86A3-40D3-AC41-9D29E0F94E53}" name="Office name" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{DE541218-B900-430B-B011-D2D8A9EDE650}" name="البريد والاتصالات السلكية واللاسلكية_x000a_Post and Telecommunications" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{2FA60EF6-F139-4108-913C-BC4C3A406E12}" name="التجارة_x000a_Commerce" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{D08A8602-96FC-41FF-AAAB-C2A1C9E294A8}" name="التشييد والبناء_x000a_Construction" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{DA1600D4-3B8C-4A29-806F-A68471F0E9D4}" name="التعدين والبترول واستغلال المحاجر_x000a_Mining and Quarrying" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{55D362D4-369B-42B5-B2EE-65BBCA2A7935}" name="الخدمات الجماعية والإجتماعية الأخرى_x000a_Community services and Other Social services" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{BA0A3B21-570C-4568-B44E-C6B9F9328E21}" name="الزراعة والصيد_x000a_Agriculture and Fishing" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{BDEDFF14-6509-4499-B370-A4E23A55246F}" name="الصناعات التحويلية_x000a_Manufacturing industries" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{627A3DC3-1C60-4D86-BC52-297920EBC51E}" name="الكهرباء والغاز والمياه_x000a_Electricity, Gas and Water" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{CC5D2944-B2A5-49D3-B79A-E30D322A1D50}" name="المال والتأمين والعقار وخدمات الاعمال_x000a_Finance, Insurance, Real estate and Business services" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{0716F104-7E06-47CC-8263-0CE618220EF0}" name="أنشطة أخرى_x000a_Other Activities" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{06EEC659-199C-42DD-9671-48D7EAA351C1}" name="اسم المكتب" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{72363C04-FB24-4800-B50A-116D69084057}" name="السنة" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{9D7B1AB2-4635-4CAD-BE08-71FA7FC8F214}" name="الربع" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{AD06DBA2-86A3-40D3-AC41-9D29E0F94E53}" name="Office name" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{DE541218-B900-430B-B011-D2D8A9EDE650}" name="البريد والاتصالات السلكية واللاسلكية_x000a_Post and Telecommunications" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{2FA60EF6-F139-4108-913C-BC4C3A406E12}" name="التجارة_x000a_Commerce" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{D08A8602-96FC-41FF-AAAB-C2A1C9E294A8}" name="التشييد والبناء_x000a_Construction" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{DA1600D4-3B8C-4A29-806F-A68471F0E9D4}" name="التعدين والبترول واستغلال المحاجر_x000a_Mining and Quarrying" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{55D362D4-369B-42B5-B2EE-65BBCA2A7935}" name="الخدمات الجماعية والإجتماعية الأخرى_x000a_Community services and Other Social services" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{BA0A3B21-570C-4568-B44E-C6B9F9328E21}" name="الزراعة والصيد_x000a_Agriculture and Fishing" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{BDEDFF14-6509-4499-B370-A4E23A55246F}" name="الصناعات التحويلية_x000a_Manufacturing industries" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{627A3DC3-1C60-4D86-BC52-297920EBC51E}" name="الكهرباء والغاز والمياه_x000a_Electricity, Gas and Water" dataDxfId="81"/>
+    <tableColumn id="10" xr3:uid="{CC5D2944-B2A5-49D3-B79A-E30D322A1D50}" name="المال والتأمين والعقار وخدمات الاعمال_x000a_Finance, Insurance, Real estate and Business services" dataDxfId="80"/>
+    <tableColumn id="11" xr3:uid="{0716F104-7E06-47CC-8263-0CE618220EF0}" name="أنشطة أخرى_x000a_Other Activities" dataDxfId="79"/>
+    <tableColumn id="12" xr3:uid="{06EEC659-199C-42DD-9671-48D7EAA351C1}" name="اسم المكتب" dataDxfId="78"/>
+    <tableColumn id="13" xr3:uid="{72363C04-FB24-4800-B50A-116D69084057}" name="السنة" dataDxfId="77"/>
+    <tableColumn id="14" xr3:uid="{9D7B1AB2-4635-4CAD-BE08-71FA7FC8F214}" name="الربع" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C74A86FA-C07E-429A-97C8-5CF6972106E0}" name="Table1" displayName="Table1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="78" dataDxfId="79" headerRowBorderDxfId="92" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C74A86FA-C07E-429A-97C8-5CF6972106E0}" name="Table1" displayName="Table1" ref="A1:N23" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72">
   <autoFilter ref="A1:N23" xr:uid="{C74A86FA-C07E-429A-97C8-5CF6972106E0}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{D69CD0AC-2A0A-46C9-9300-1FB9F25C60E2}" name="Office name" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{15719876-10DB-4116-A589-510D24A638F6}" name="الاختصاصيون في المواضيع العلمية والفنية والإنسانية_x000a_Specialists in scientific, technical and humanity subject" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{5700715A-1CBA-4BFB-B8F1-8D8414E7DAE1}" name="الفنيون في المواضيع العلمية والفنية والإنسانية_x000a_Technicians in scientific, technical and humanity subject" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{68324B02-9678-460B-BF3A-FF6C736D0321}" name="المهن الكتابية_x000a_Clerical occupations" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{69FF956D-CD18-49DC-AB7E-D8A7ECB8D88D}" name="المهن الهندسية الأساسية المساعدة_x000a_Basic engineering professions" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{679F43CE-E92A-41B4-8786-4EFEDA4B2111}" name="المديرون ومديرو الأعمال_x000a_Managers and business managers" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{E21ED83D-0AAA-4AA3-8D0F-C164568484BF}" name="مهن البيع_x000a_Sales occupations" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{C777E4FC-BFA5-46EC-BE19-2C72760513FE}" name="مهن الخدمات_x000a_Service occupations" dataDxfId="84"/>
-    <tableColumn id="9" xr3:uid="{D5D74D3F-471C-443C-9591-6265ED312F55}" name="مهن الزراعة والصيد وتربية الحيوان والطيور_x000a_Agriculture, hunting and animal husbandry" dataDxfId="83"/>
-    <tableColumn id="10" xr3:uid="{0FF06985-3ECC-4B8A-ABEC-8FFD9ECEA7D5}" name="مهن العمليات الصناعية والكيميائية والصناعات الغذائية_x000a_Industrial/chemical processes and food industries" dataDxfId="82"/>
-    <tableColumn id="11" xr3:uid="{4C064CC4-15D8-4C8F-BAD5-B1BBEB0F69E3}" name="مهن أخرى_x000a_Other occupations" dataDxfId="81"/>
-    <tableColumn id="12" xr3:uid="{8D8D57E5-EDC8-42BA-AD03-FF8E9AF97C25}" name="اسم المكتب" dataDxfId="80"/>
-    <tableColumn id="13" xr3:uid="{C5FCCC98-5523-4617-B30E-499A284D6024}" name="السنة" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{3E527ECD-52C9-4443-ADA0-1194E8FE0A4D}" name="الربع" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{D69CD0AC-2A0A-46C9-9300-1FB9F25C60E2}" name="Office name" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{15719876-10DB-4116-A589-510D24A638F6}" name="الاختصاصيون في المواضيع العلمية والفنية والإنسانية_x000a_Specialists in scientific, technical and humanity subject" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{5700715A-1CBA-4BFB-B8F1-8D8414E7DAE1}" name="الفنيون في المواضيع العلمية والفنية والإنسانية_x000a_Technicians in scientific, technical and humanity subject" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{68324B02-9678-460B-BF3A-FF6C736D0321}" name="المهن الكتابية_x000a_Clerical occupations" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{69FF956D-CD18-49DC-AB7E-D8A7ECB8D88D}" name="المهن الهندسية الأساسية المساعدة_x000a_Basic engineering professions" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{679F43CE-E92A-41B4-8786-4EFEDA4B2111}" name="المديرون ومديرو الأعمال_x000a_Managers and business managers" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{E21ED83D-0AAA-4AA3-8D0F-C164568484BF}" name="مهن البيع_x000a_Sales occupations" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{C777E4FC-BFA5-46EC-BE19-2C72760513FE}" name="مهن الخدمات_x000a_Service occupations" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{D5D74D3F-471C-443C-9591-6265ED312F55}" name="مهن الزراعة والصيد وتربية الحيوان والطيور_x000a_Agriculture, hunting and animal husbandry" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{0FF06985-3ECC-4B8A-ABEC-8FFD9ECEA7D5}" name="مهن العمليات الصناعية والكيميائية والصناعات الغذائية_x000a_Industrial/chemical processes and food industries" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{4C064CC4-15D8-4C8F-BAD5-B1BBEB0F69E3}" name="مهن أخرى_x000a_Other occupations" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{8D8D57E5-EDC8-42BA-AD03-FF8E9AF97C25}" name="اسم المكتب" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{C5FCCC98-5523-4617-B30E-499A284D6024}" name="السنة" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{3E527ECD-52C9-4443-ADA0-1194E8FE0A4D}" name="الربع" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D80739B4-998F-4100-A1A8-BD9C53D3F3BF}" name="Table3" displayName="Table3" ref="A1:H23" totalsRowShown="0" headerRowDxfId="52" dataDxfId="53" headerRowBorderDxfId="60" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D80739B4-998F-4100-A1A8-BD9C53D3F3BF}" name="Table3" displayName="Table3" ref="A1:H23" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
   <autoFilter ref="A1:H23" xr:uid="{D80739B4-998F-4100-A1A8-BD9C53D3F3BF}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CE8A8F00-ED61-4C3F-83C5-B5F619D97BA0}" name="Office name" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{BAFAC399-15C7-4480-8482-9275FCCA854C}" name="شفاء بدون عجز_x000a_Cured Without Disability" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{394C14A0-F0D1-404D-A43C-50E4C0FE8CF9}" name="شفاء بعجز_x000a_Cured With Disability" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{83733EEB-1B80-421D-BA1A-6035FFE1FAD3}" name="وفاة_x000a_Death" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{AAE382E0-EDC7-4776-AE0B-AC336DE41368}" name="تحت العلاج_x000a_Under recovery" dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{9D304F0E-CC3A-45F9-8B91-900A87DB6D74}" name="اسم المكتب" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{ED369971-527F-4E75-9613-1529169703A9}" name="السنة" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{B97736BC-049B-463A-AB02-78BB6F8D307D}" name="الربع" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{CE8A8F00-ED61-4C3F-83C5-B5F619D97BA0}" name="Office name" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{BAFAC399-15C7-4480-8482-9275FCCA854C}" name="شفاء بدون عجز_x000a_Cured Without Disability" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{394C14A0-F0D1-404D-A43C-50E4C0FE8CF9}" name="شفاء بعجز_x000a_Cured With Disability" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{83733EEB-1B80-421D-BA1A-6035FFE1FAD3}" name="وفاة_x000a_Death" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{AAE382E0-EDC7-4776-AE0B-AC336DE41368}" name="تحت العلاج_x000a_Under recovery" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{9D304F0E-CC3A-45F9-8B91-900A87DB6D74}" name="اسم المكتب" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{ED369971-527F-4E75-9613-1529169703A9}" name="السنة" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{B97736BC-049B-463A-AB02-78BB6F8D307D}" name="الربع" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E755595D-C9E7-47B1-91F2-FF3EB8095E97}" name="Table4" displayName="Table4" ref="A1:H23" totalsRowShown="0" headerRowBorderDxfId="50" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E755595D-C9E7-47B1-91F2-FF3EB8095E97}" name="Table4" displayName="Table4" ref="A1:H23" totalsRowShown="0" headerRowBorderDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A1:H23" xr:uid="{E755595D-C9E7-47B1-91F2-FF3EB8095E97}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F8375460-A989-440E-BC4B-8B2D9EC7019B}" name="Office name" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{B9A8FBB4-3DEB-43BF-A958-535B10970285}" name="Saudi-Male" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{C3F9482F-809B-4338-9D81-D9ABDE37A1FE}" name="Saudi-Female" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{CBE09EA5-2BC5-4028-833B-9E79B5AA0FED}" name="Non-Saudi-Male" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{9B90D070-E62F-49B5-848D-1C1076041163}" name="Non-Saudi-Female" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{3E0018A2-836A-4D20-AAED-BB68553E228B}" name="اسم المكتب" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{EEF9E858-8168-4043-92CD-E6CEA6660E92}" name="السنة" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{AEDA96FC-E4CB-41DB-AE20-8A832A59DF7F}" name="الربع" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{F8375460-A989-440E-BC4B-8B2D9EC7019B}" name="Office name" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{B9A8FBB4-3DEB-43BF-A958-535B10970285}" name="Saudi-Male" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{C3F9482F-809B-4338-9D81-D9ABDE37A1FE}" name="Saudi-Female" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{CBE09EA5-2BC5-4028-833B-9E79B5AA0FED}" name="Non-Saudi-Male" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{9B90D070-E62F-49B5-848D-1C1076041163}" name="Non-Saudi-Female" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{3E0018A2-836A-4D20-AAED-BB68553E228B}" name="اسم المكتب" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{EEF9E858-8168-4043-92CD-E6CEA6660E92}" name="السنة" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{AEDA96FC-E4CB-41DB-AE20-8A832A59DF7F}" name="الربع" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357B0EE9-6728-4E4C-BA81-27AF793832C7}" name="Table5" displayName="Table5" ref="A1:N23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="29" headerRowBorderDxfId="42" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357B0EE9-6728-4E4C-BA81-27AF793832C7}" name="Table5" displayName="Table5" ref="A1:N23" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
   <autoFilter ref="A1:N23" xr:uid="{357B0EE9-6728-4E4C-BA81-27AF793832C7}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{AD8847AC-88F8-4083-955A-96B07784F99F}" name="Office name" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{D438583D-4DDE-470D-A4D7-42736FFB9483}" name="الاحتجاز_x000a_CAUGHT IN" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{0DC8EA2B-DF76-4F95-927A-83D307F96E12}" name="الارتطام أو الاصطدام_x000a_Struck and Collision" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{E9A73B82-BAF3-42D0-921F-77C720458EC5}" name="الحك أو الكشط_x000a_Rubbed and Abrasion" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{ED2C4D52-A0FE-4054-811B-229EBDD783EC}" name="السقوط_x000a_Fall" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{581F2D7B-27B3-4259-8332-C0932FB41DF9}" name="حوادث النقل والسيارات_x000a_ Transport and car Accidents" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{BC84DD86-8532-4E43-8FF5-2AF420FF1D15}" name="الاجهاد المفرط_x000a_OVERE" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{6E2EBA06-FC0A-464B-BDFB-74B1C5C2C48D}" name="رد الفعل الجسدي_x000a_BODILY REACTION" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{3EF885B6-E9F9-448F-8E1F-AE64C017C4E1}" name="التلامس بالبرودة أو الحرارة_x000a_CONTACT WITH TEMPERATURE EXTREMES" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{F20283A7-DD7D-40BA-BF61-36D96271D244}" name="التلامس بالاشعاعات أو الكاويات_x000a_CONTACT WITH RADIATION and CAUSTICS" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{658BA30C-8DCA-4C94-8EBC-55BC9EE4091D}" name="أسباب أخرى_x000a_Other Accidents" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{B8B6344E-21A6-4BE3-AD44-7ADDE241905F}" name="اسم المكتب" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{D071FD8E-E942-473C-AFE2-CE92F1995DC1}" name="السنة" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{6C18FC6D-440B-4C56-B3B9-5CBFD3C01E8F}" name="الربع" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{AD8847AC-88F8-4083-955A-96B07784F99F}" name="Office name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{D438583D-4DDE-470D-A4D7-42736FFB9483}" name="الاحتجاز_x000a_CAUGHT IN" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{0DC8EA2B-DF76-4F95-927A-83D307F96E12}" name="الارتطام أو الاصطدام_x000a_Struck and Collision" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E9A73B82-BAF3-42D0-921F-77C720458EC5}" name="الحك أو الكشط_x000a_Rubbed and Abrasion" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{ED2C4D52-A0FE-4054-811B-229EBDD783EC}" name="السقوط_x000a_Fall" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{581F2D7B-27B3-4259-8332-C0932FB41DF9}" name="حوادث النقل والسيارات_x000a_ Transport and car Accidents" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{BC84DD86-8532-4E43-8FF5-2AF420FF1D15}" name="الاجهاد المفرط_x000a_OVERE" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{6E2EBA06-FC0A-464B-BDFB-74B1C5C2C48D}" name="رد الفعل الجسدي_x000a_BODILY REACTION" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{3EF885B6-E9F9-448F-8E1F-AE64C017C4E1}" name="التلامس بالبرودة أو الحرارة_x000a_CONTACT WITH TEMPERATURE EXTREMES" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{F20283A7-DD7D-40BA-BF61-36D96271D244}" name="التلامس بالاشعاعات أو الكاويات_x000a_CONTACT WITH RADIATION and CAUSTICS" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{658BA30C-8DCA-4C94-8EBC-55BC9EE4091D}" name="أسباب أخرى_x000a_Other Accidents" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{B8B6344E-21A6-4BE3-AD44-7ADDE241905F}" name="اسم المكتب" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{D071FD8E-E942-473C-AFE2-CE92F1995DC1}" name="السنة" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{6C18FC6D-440B-4C56-B3B9-5CBFD3C01E8F}" name="الربع" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE9C9622-0EF5-4580-88AE-DAFE82504C52}" name="Table6" displayName="Table6" ref="B1:O23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13" headerRowBorderDxfId="26" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE9C9622-0EF5-4580-88AE-DAFE82504C52}" name="Table6" displayName="Table6" ref="B1:O23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="B1:O23" xr:uid="{BE9C9622-0EF5-4580-88AE-DAFE82504C52}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{9DC31FD8-DBAA-4431-9969-EDFF286931CF}" name="Office name" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4578D935-9957-4830-9EE7-61E491D2BB74}" name="15 ~ 19" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{ABDA58BC-F1CA-41A0-B409-8A1C8ABFE143}" name="20 ~ 24" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{58FD605D-72F1-473B-9425-43E84E50E442}" name="25 ~ 29" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{9AF0CC54-D35D-4ADA-B4B3-F24093254850}" name="30 ~ 34" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{665E1F8E-6353-42B3-BFCB-70D03BDB608E}" name="35 ~ 39" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{B641EDF2-73DC-49A3-BF71-A2520EFFCC06}" name="40 ~ 44" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{EFB352C7-A38A-4883-AD75-C777E1DE7559}" name="45 ~ 49" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{DE579992-D7B2-4BCE-BD72-3342040D7193}" name="50 ~ 54" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{08255EFA-AA04-4B94-BC10-75B501E1B1A5}" name="55 ~ 59" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{14EC699C-5476-404E-A4B3-5EAC8D0534A4}" name="&gt;= 60" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{C515C878-A997-45DA-AE5B-14579329674E}" name="اسم المكتب" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{0B6AE3E0-1BFD-477B-9FBB-5AD0B4A4D638}" name="السنة" dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{84849AC5-B8C5-4553-8B54-EE8231085275}" name="الربع" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9DC31FD8-DBAA-4431-9969-EDFF286931CF}" name="Office name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4578D935-9957-4830-9EE7-61E491D2BB74}" name="15 ~ 19" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{ABDA58BC-F1CA-41A0-B409-8A1C8ABFE143}" name="20 ~ 24" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{58FD605D-72F1-473B-9425-43E84E50E442}" name="25 ~ 29" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{9AF0CC54-D35D-4ADA-B4B3-F24093254850}" name="30 ~ 34" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{665E1F8E-6353-42B3-BFCB-70D03BDB608E}" name="35 ~ 39" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{B641EDF2-73DC-49A3-BF71-A2520EFFCC06}" name="40 ~ 44" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{EFB352C7-A38A-4883-AD75-C777E1DE7559}" name="45 ~ 49" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{DE579992-D7B2-4BCE-BD72-3342040D7193}" name="50 ~ 54" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{08255EFA-AA04-4B94-BC10-75B501E1B1A5}" name="55 ~ 59" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{14EC699C-5476-404E-A4B3-5EAC8D0534A4}" name="&gt;= 60" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C515C878-A997-45DA-AE5B-14579329674E}" name="اسم المكتب" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{0B6AE3E0-1BFD-477B-9FBB-5AD0B4A4D638}" name="السنة" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{84849AC5-B8C5-4553-8B54-EE8231085275}" name="الربع" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4537,7 +4537,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="71.400000000000006" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -5673,8 +5673,7 @@
     <col min="12" max="12" width="29" style="11" customWidth="1"/>
     <col min="13" max="13" width="29" style="46" customWidth="1"/>
     <col min="14" max="14" width="22.19921875" style="12" customWidth="1"/>
-    <col min="15" max="16" width="0" style="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0" style="11" hidden="1"/>
+    <col min="15" max="17" width="0" style="11" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="9" style="11" hidden="1"/>
   </cols>
   <sheetData>
@@ -7614,10 +7613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.09765625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -8244,7 +8243,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:XFD40"/>
+  <dimension ref="A1:XFC40"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:N23"/>
@@ -9529,7 +9528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -11188,10 +11187,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ItemName xmlns="f343b1d2-c951-4356-b116-187ff6b1ca69">31</ItemName>
@@ -11200,7 +11195,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="مستند" ma:contentTypeID="0x01010030171DDB5196394781920AFBF200A239" ma:contentTypeVersion="3" ma:contentTypeDescription="إنشاء مستند جديد." ma:contentTypeScope="" ma:versionID="7025881ddbd734274ee6de91e434df03">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f343b1d2-c951-4356-b116-187ff6b1ca69" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32546d60ee5875e7e04058d7eebc7be3" ns2:_="">
     <xsd:import namespace="f343b1d2-c951-4356-b116-187ff6b1ca69"/>
@@ -11338,24 +11346,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E97DC769-6EEA-4B35-8112-79ABAAE26CA6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B0C819-8A2D-42C5-BF89-D02F81F7D57A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11365,7 +11356,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E97DC769-6EEA-4B35-8112-79ABAAE26CA6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5932EC5-E05C-4D7C-B663-D4D56176CE7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D89000F2-F4A3-4FCE-BD68-C6DA5A5CD228}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11381,12 +11388,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5932EC5-E05C-4D7C-B663-D4D56176CE7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>